<commit_message>
first round of combustion
</commit_message>
<xml_diff>
--- a/pressuretemps.xlsx
+++ b/pressuretemps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\embas\Documents\GitHub\Thermal-Fluids-Gas-Turbine-Simulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183E367A-3A1A-458B-B6F7-2A3A65470515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715DFEB9-E931-4D29-A6E9-18C8C52D6E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7237" yWindow="3360" windowWidth="16200" windowHeight="9308" xr2:uid="{E298BD80-BBB2-4960-ABED-8A50683300C2}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{E298BD80-BBB2-4960-ABED-8A50683300C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>TempK</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>PressBar</t>
+  </si>
+  <si>
+    <t>PresskPa</t>
   </si>
 </sst>
 </file>
@@ -416,15 +419,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06677396-8161-4994-A1E1-605006ADC3BE}">
-  <dimension ref="B2:D26"/>
+  <dimension ref="B2:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -434,8 +437,11 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B3">
         <v>0.01</v>
       </c>
@@ -446,8 +452,12 @@
       <c r="D3">
         <v>6.11E-3</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="E3">
+        <f>D3*100</f>
+        <v>0.61099999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B4">
         <v>10</v>
       </c>
@@ -458,8 +468,12 @@
       <c r="D4">
         <v>1.2279999999999999E-2</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="E4">
+        <f t="shared" ref="E4:E26" si="1">D4*100</f>
+        <v>1.228</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B5">
         <v>20</v>
       </c>
@@ -470,8 +484,12 @@
       <c r="D5">
         <v>2.3390000000000001E-2</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>2.339</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B6">
         <v>30</v>
       </c>
@@ -482,8 +500,12 @@
       <c r="D6">
         <v>4.2459999999999998E-2</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>4.2459999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B7">
         <v>40</v>
       </c>
@@ -494,8 +516,12 @@
       <c r="D7">
         <v>7.3840000000000003E-2</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>7.3840000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B8">
         <v>50</v>
       </c>
@@ -506,8 +532,12 @@
       <c r="D8">
         <v>0.1235</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>12.35</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B9">
         <v>60</v>
       </c>
@@ -518,8 +548,12 @@
       <c r="D9">
         <v>0.19939999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>19.939999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B10">
         <v>70</v>
       </c>
@@ -530,8 +564,12 @@
       <c r="D10">
         <v>0.31190000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>31.19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B11">
         <v>80</v>
       </c>
@@ -542,8 +580,12 @@
       <c r="D11">
         <v>0.47389999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>47.39</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B12">
         <v>90</v>
       </c>
@@ -554,8 +596,12 @@
       <c r="D12">
         <v>0.70140000000000002</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>70.14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B13">
         <v>100</v>
       </c>
@@ -566,8 +612,12 @@
       <c r="D13">
         <v>1.014</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>101.4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B14">
         <v>120</v>
       </c>
@@ -578,8 +628,12 @@
       <c r="D14">
         <v>1.9850000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>198.5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B15">
         <v>140</v>
       </c>
@@ -590,8 +644,12 @@
       <c r="D15">
         <v>3.613</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>361.3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B16">
         <v>160</v>
       </c>
@@ -602,8 +660,12 @@
       <c r="D16">
         <v>6.1779999999999999</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>617.79999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B17">
         <v>180</v>
       </c>
@@ -614,8 +676,12 @@
       <c r="D17">
         <v>10.02</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B18">
         <v>200</v>
       </c>
@@ -626,8 +692,12 @@
       <c r="D18">
         <v>15.54</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B19">
         <v>220</v>
       </c>
@@ -638,8 +708,12 @@
       <c r="D19">
         <v>23.18</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>2318</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B20">
         <v>240</v>
       </c>
@@ -650,8 +724,12 @@
       <c r="D20">
         <v>33.44</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>3344</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B21">
         <v>260</v>
       </c>
@@ -662,8 +740,12 @@
       <c r="D21">
         <v>46.88</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>4688</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B22">
         <v>280</v>
       </c>
@@ -674,8 +756,12 @@
       <c r="D22">
         <v>64.12</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>6412</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B23">
         <v>300</v>
       </c>
@@ -686,8 +772,12 @@
       <c r="D23">
         <v>85.81</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>8581</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B24">
         <v>320</v>
       </c>
@@ -698,8 +788,12 @@
       <c r="D24">
         <v>112.7</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>11270</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B25">
         <v>340</v>
       </c>
@@ -710,8 +804,12 @@
       <c r="D25">
         <v>145.9</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>14590</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B26">
         <v>360</v>
       </c>
@@ -721,6 +819,10 @@
       </c>
       <c r="D26">
         <v>186.5</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>18650</v>
       </c>
     </row>
   </sheetData>

</xml_diff>